<commit_message>
remove Report-No from Excel-Template
</commit_message>
<xml_diff>
--- a/excel/Template.xlsx
+++ b/excel/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerhard\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jona\Documents\art\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3993586-ED85-4D7B-9E9A-1A19A1B14E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5625B3F0-FA87-4D13-BF23-1DAF2DE63A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -488,7 +491,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Datum" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -559,7 +562,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -881,11 +884,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:J56"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
@@ -980,9 +983,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="24"/>
-      <c r="C7" s="25">
-        <v>93</v>
-      </c>
+      <c r="C7" s="25"/>
       <c r="D7" s="23" t="s">
         <v>2</v>
       </c>

</xml_diff>